<commit_message>
September 25 2020: Added automatic formatting of results
</commit_message>
<xml_diff>
--- a/2020_09_25/2020-09-25.xlsx
+++ b/2020_09_25/2020-09-25.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="258" uniqueCount="258">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="279" uniqueCount="258">
   <si>
     <t xml:space="preserve">A database resource for Genome-wide dynamics analysis of Coronaviruses on a historical and global scale</t>
   </si>
@@ -88,709 +88,709 @@
     <t xml:space="preserve">The IMEx Coronavirus interactome: an evolving map of Coronaviridae-Host molecular interactions</t>
   </si>
   <si>
+    <t xml:space="preserve">https://doi.org/10.1101/2020.06.16.153817</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A systems approach to inflammation identifies therapeutic targets in SARS-CoV-2 infection</t>
+  </si>
+  <si>
     <t xml:space="preserve">2020-05-24</t>
   </si>
   <si>
-    <t xml:space="preserve">https://doi.org/10.1101/2020.06.16.153817</t>
-  </si>
-  <si>
-    <t xml:space="preserve">A systems approach to inflammation identifies therapeutic targets in SARS-CoV-2 infection</t>
+    <t xml:space="preserve">https://doi.org/10.1101/2020.05.23.20110916</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Comparative multiplexed interactomics of SARS-CoV-2 and homologous coronavirus non-structural proteins identifies unique and shared host-cell dependencies</t>
   </si>
   <si>
     <t xml:space="preserve">2020-07-15</t>
   </si>
   <si>
-    <t xml:space="preserve">https://doi.org/10.1101/2020.05.23.20110916</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Comparative multiplexed interactomics of SARS-CoV-2 and homologous coronavirus non-structural proteins identifies unique and shared host-cell dependencies</t>
+    <t xml:space="preserve">https://doi.org/10.1101/2020.07.13.201517</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A distinct innate immune signature marks progression from mild to severe COVID-19</t>
   </si>
   <si>
     <t xml:space="preserve">2020-08-04</t>
   </si>
   <si>
-    <t xml:space="preserve">https://doi.org/10.1101/2020.07.13.201517</t>
-  </si>
-  <si>
-    <t xml:space="preserve">A distinct innate immune signature marks progression from mild to severe COVID-19</t>
+    <t xml:space="preserve">https://doi.org/10.1101/2020.08.04.236315</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Discovery of drugs to treat cytokine storm-induced cardiac dysfunction using human cardiac organoids</t>
   </si>
   <si>
     <t xml:space="preserve">2020-08-24</t>
   </si>
   <si>
-    <t xml:space="preserve">https://doi.org/10.1101/2020.08.04.236315</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Discovery of drugs to treat cytokine storm-induced cardiac dysfunction using human cardiac organoids</t>
+    <t xml:space="preserve">https://doi.org/10.1101/2020.08.23.258574</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Versatile, Multivalent Nanobody Cocktails for Highly Efficient SARS-CoV-2 Neutralization</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://doi.org/10.1101/2020.08.24.264333</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Evidence for structural protein damage and membrane lipid remodeling in red blood cells from COVID-19 patients</t>
   </si>
   <si>
     <t xml:space="preserve">2020-06-30</t>
   </si>
   <si>
-    <t xml:space="preserve">https://doi.org/10.1101/2020.08.23.258574</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Versatile, Multivalent Nanobody Cocktails for Highly Efficient SARS-CoV-2 Neutralization</t>
+    <t xml:space="preserve">https://doi.org/10.1101/2020.06.29.20142703</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SARS-CoV-2 proteome microarray for mapping COVID-19 antibody interactions at amino acid resolution</t>
   </si>
   <si>
     <t xml:space="preserve">2020-03-28</t>
   </si>
   <si>
-    <t xml:space="preserve">https://doi.org/10.1101/2020.08.24.264333</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Evidence for structural protein damage and membrane lipid remodeling in red blood cells from COVID-19 patients</t>
+    <t xml:space="preserve">https://doi.org/10.1101/2020.03.26.994756</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Re-analysis of SARS-CoV-2 infected host cell proteomics time-course data by impact pathway analysis and network analysis. A potential link with inflammatory response.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://doi.org/10.1101/2020.03.26.009605</t>
+  </si>
+  <si>
+    <t xml:space="preserve">In silico approach to accelerate the development of mass spectrometry-based proteomics methods for detection of viral proteins: Application to COVID-19</t>
   </si>
   <si>
     <t xml:space="preserve">2020-03-10</t>
   </si>
   <si>
-    <t xml:space="preserve">https://doi.org/10.1101/2020.06.29.20142703</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SARS-CoV-2 proteome microarray for mapping COVID-19 antibody interactions at amino acid resolution</t>
+    <t xml:space="preserve">https://doi.org/10.1101/2020.03.08.980383</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Assignment of coronavirus spike protein site-specific glycosylation using GlycReSoft</t>
   </si>
   <si>
     <t xml:space="preserve">2020-05-31</t>
   </si>
   <si>
-    <t xml:space="preserve">https://doi.org/10.1101/2020.03.26.994756</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Re-analysis of SARS-CoV-2 infected host cell proteomics time-course data by impact pathway analysis and network analysis. A potential link with inflammatory response.</t>
+    <t xml:space="preserve">https://doi.org/10.1101/2020.05.31.125302</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Suppressive myeloid cells are a hallmark of severe COVID-19</t>
   </si>
   <si>
     <t xml:space="preserve">2020-06-05</t>
   </si>
   <si>
-    <t xml:space="preserve">https://doi.org/10.1101/2020.03.26.009605</t>
-  </si>
-  <si>
-    <t xml:space="preserve">In silico approach to accelerate the development of mass spectrometry-based proteomics methods for detection of viral proteins: Application to COVID-19</t>
+    <t xml:space="preserve">https://doi.org/10.1101/2020.06.03.20119818</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Candidate screening of host cell membrane proteins involved in SARS-CoV-2 entry</t>
   </si>
   <si>
     <t xml:space="preserve">2020-09-09</t>
   </si>
   <si>
-    <t xml:space="preserve">https://doi.org/10.1101/2020.03.08.980383</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Assignment of coronavirus spike protein site-specific glycosylation using GlycReSoft</t>
+    <t xml:space="preserve">https://doi.org/10.1101/2020.09.09.289488</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ALTERED MOLECULAR PATHWAYS OBSERVED IN NASO-OROPHARYNGEAL SAMPLES OF SARS-CoV-2 PATIENTS</t>
   </si>
   <si>
     <t xml:space="preserve">2020-05-18</t>
   </si>
   <si>
-    <t xml:space="preserve">https://doi.org/10.1101/2020.05.31.125302</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Suppressive myeloid cells are a hallmark of severe COVID-19</t>
+    <t xml:space="preserve">https://doi.org/10.1101/2020.05.14.20102558</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Serum protein profiling reveals a landscape of inflammation and immune signaling in early-stage COVID-19 infection</t>
   </si>
   <si>
     <t xml:space="preserve">2020-05-13</t>
   </si>
   <si>
-    <t xml:space="preserve">https://doi.org/10.1101/2020.06.03.20119818</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Candidate screening of host cell membrane proteins involved in SARS-CoV-2 entry</t>
+    <t xml:space="preserve">https://doi.org/10.1101/2020.05.08.20095836</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SARS-CoV-2 Nucleocapsid protein is decorated with multiple N- and O-glycans.</t>
   </si>
   <si>
     <t xml:space="preserve">2020-08-27</t>
   </si>
   <si>
-    <t xml:space="preserve">https://doi.org/10.1101/2020.09.09.289488</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ALTERED MOLECULAR PATHWAYS OBSERVED IN NASO-OROPHARYNGEAL SAMPLES OF SARS-CoV-2 PATIENTS</t>
+    <t xml:space="preserve">https://doi.org/10.1101/2020.08.26.269043</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Exploring diseases/traits and blood proteins causally related to expression of ACE2, the putative receptor of 2019-nCov: A Mendelian Randomization analysis</t>
   </si>
   <si>
     <t xml:space="preserve">2020-03-08</t>
   </si>
   <si>
-    <t xml:space="preserve">https://doi.org/10.1101/2020.05.14.20102558</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Serum protein profiling reveals a landscape of inflammation and immune signaling in early-stage COVID-19 infection</t>
+    <t xml:space="preserve">https://doi.org/10.1101/2020.03.04.20031237</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Distinct early IgA profile may determine severity of COVID-19 symptoms: an immunological case series</t>
   </si>
   <si>
     <t xml:space="preserve">2020-04-17</t>
   </si>
   <si>
-    <t xml:space="preserve">https://doi.org/10.1101/2020.05.08.20095836</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SARS-CoV-2 Nucleocapsid protein is decorated with multiple N- and O-glycans.</t>
+    <t xml:space="preserve">https://doi.org/10.1101/2020.04.14.20059733</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sampling SARS-CoV-2 proteomes for predicted CD8 T-cell epitopes as a tool for understanding immunogenic breadth and rationale vaccine design</t>
   </si>
   <si>
     <t xml:space="preserve">2020-08-16</t>
   </si>
   <si>
-    <t xml:space="preserve">https://doi.org/10.1101/2020.08.26.269043</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Exploring diseases/traits and blood proteins causally related to expression of ACE2, the putative receptor of 2019-nCov: A Mendelian Randomization analysis</t>
+    <t xml:space="preserve">https://doi.org/10.1101/2020.08.15.250647</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Artificial intelligence predicts the immunogenic landscape of SARS-CoV-2: toward universal blueprints for vaccine designs</t>
   </si>
   <si>
     <t xml:space="preserve">2020-04-21</t>
   </si>
   <si>
-    <t xml:space="preserve">https://doi.org/10.1101/2020.03.04.20031237</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Distinct early IgA profile may determine severity of COVID-19 symptoms: an immunological case series</t>
+    <t xml:space="preserve">https://doi.org/10.1101/2020.04.21.052084</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Global variation in the SARS-CoV-2 proteome reveals the mutational hotspots in the drug and vaccine candidates</t>
   </si>
   <si>
     <t xml:space="preserve">2020-07-31</t>
   </si>
   <si>
-    <t xml:space="preserve">https://doi.org/10.1101/2020.04.14.20059733</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sampling SARS-CoV-2 proteomes for predicted CD8 T-cell epitopes as a tool for understanding immunogenic breadth and rationale vaccine design</t>
+    <t xml:space="preserve">https://doi.org/10.1101/2020.07.31.230987</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Immunoinformatic identification of B cell and T cell epitopes in the SARS-CoV-2 proteome</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://doi.org/10.1101/2020.05.14.093757</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Global BioID-based SARS-CoV-2 proteins proximal interactome unveils novel ties between viral polypeptides and host factors involved in multiple COVID19-associated mechanisms</t>
   </si>
   <si>
     <t xml:space="preserve">2020-08-29</t>
   </si>
   <si>
-    <t xml:space="preserve">https://doi.org/10.1101/2020.08.15.250647</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Artificial intelligence predicts the immunogenic landscape of SARS-CoV-2: toward universal blueprints for vaccine designs</t>
+    <t xml:space="preserve">https://doi.org/10.1101/2020.08.28.272955</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Secondary analysis of transcriptomes of SARS-CoV-2 infection models to characterize COVID-19</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://doi.org/10.1101/2020.08.27.270835</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ReScan, a Multiplex Diagnostic Pipeline, Pans Human Sera for SARS-CoV-2 Antigens</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://doi.org/10.1101/2020.05.11.20092528</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Antibody dynamics to SARS-CoV-2 in Asymptomatic and Mild COVID-19 patients</t>
   </si>
   <si>
     <t xml:space="preserve">2020-07-11</t>
   </si>
   <si>
-    <t xml:space="preserve">https://doi.org/10.1101/2020.04.21.052084</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Global variation in the SARS-CoV-2 proteome reveals the mutational hotspots in the drug and vaccine candidates</t>
+    <t xml:space="preserve">https://doi.org/10.1101/2020.07.09.20149633</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Multi-level proteomics reveals host-perturbation strategies of SARS-CoV-2 and SARS-CoV</t>
   </si>
   <si>
     <t xml:space="preserve">2020-06-17</t>
   </si>
   <si>
-    <t xml:space="preserve">https://doi.org/10.1101/2020.07.31.230987</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Immunoinformatic identification of B cell and T cell epitopes in the SARS-CoV-2 proteome</t>
+    <t xml:space="preserve">https://doi.org/10.1101/2020.06.17.156455</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Proteome-wide analysis of differentially-expressed SARS-CoV-2 antibodies in early COVID-19 infection</t>
   </si>
   <si>
     <t xml:space="preserve">2020-04-20</t>
   </si>
   <si>
-    <t xml:space="preserve">https://doi.org/10.1101/2020.05.14.093757</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Global BioID-based SARS-CoV-2 proteins proximal interactome unveils novel ties between viral polypeptides and host factors involved in multiple COVID19-associated mechanisms</t>
+    <t xml:space="preserve">https://doi.org/10.1101/2020.04.14.20064535</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Common low complexity regions for SARS-CoV-2 and human proteomes as potential multidirectional risk factor in vaccine development</t>
   </si>
   <si>
     <t xml:space="preserve">2020-08-11</t>
   </si>
   <si>
-    <t xml:space="preserve">https://doi.org/10.1101/2020.08.28.272955</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Secondary analysis of transcriptomes of SARS-CoV-2 infection models to characterize COVID-19</t>
+    <t xml:space="preserve">https://doi.org/10.1101/2020.08.11.245993</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A SARS-CoV-2 Vaccination Strategy Focused on Population-Scale Immunity</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://doi.org/10.1101/2020.03.31.018978</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SARS-CoV2 (COVID-19) Structural/Evolution Dynamicome: Insights into functional evolution and human genomics.</t>
   </si>
   <si>
     <t xml:space="preserve">2020-05-15</t>
   </si>
   <si>
-    <t xml:space="preserve">https://doi.org/10.1101/2020.08.27.270835</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ReScan, a Multiplex Diagnostic Pipeline, Pans Human Sera for SARS-CoV-2 Antigens</t>
+    <t xml:space="preserve">https://doi.org/10.1101/2020.05.15.098616</t>
+  </si>
+  <si>
+    <t xml:space="preserve">COVID-19 coronavirus vaccine design using reverse vaccinology and machine learning</t>
   </si>
   <si>
     <t xml:space="preserve">2020-03-21</t>
   </si>
   <si>
-    <t xml:space="preserve">https://doi.org/10.1101/2020.05.11.20092528</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Antibody dynamics to SARS-CoV-2 in Asymptomatic and Mild COVID-19 patients</t>
+    <t xml:space="preserve">https://doi.org/10.1101/2020.03.20.000141</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Inhibiting coronavirus replication in cultured cells by chemical ER stress</t>
   </si>
   <si>
     <t xml:space="preserve">2020-08-26</t>
   </si>
   <si>
-    <t xml:space="preserve">https://doi.org/10.1101/2020.07.09.20149633</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Multi-level proteomics reveals host-perturbation strategies of SARS-CoV-2 and SARS-CoV</t>
+    <t xml:space="preserve">https://doi.org/10.1101/2020.08.26.266304</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Relevance of enriched expression of SARS-CoV-2 binding receptor ACE2 in gastrointestinal tissue with pathogenesis of digestive symptoms, diabetes-associated mortality, and disease recurrence in COVID-19 patients</t>
   </si>
   <si>
     <t xml:space="preserve">2020-04-15</t>
   </si>
   <si>
-    <t xml:space="preserve">https://doi.org/10.1101/2020.06.17.156455</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Proteome-wide analysis of differentially-expressed SARS-CoV-2 antibodies in early COVID-19 infection</t>
+    <t xml:space="preserve">https://doi.org/10.1101/2020.04.14.040204</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Global profiling of SARS-CoV-2 specific IgG/ IgM responses of convalescents using a proteome microarray</t>
   </si>
   <si>
     <t xml:space="preserve">2020-03-27</t>
   </si>
   <si>
-    <t xml:space="preserve">https://doi.org/10.1101/2020.04.14.20064535</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Common low complexity regions for SARS-CoV-2 and human proteomes as potential multidirectional risk factor in vaccine development</t>
+    <t xml:space="preserve">https://doi.org/10.1101/2020.03.20.20039495</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dark proteome of Newly Emerged SARS-CoV-2 in Comparison with Human and Bat Coronaviruses</t>
   </si>
   <si>
     <t xml:space="preserve">2020-03-14</t>
   </si>
   <si>
-    <t xml:space="preserve">https://doi.org/10.1101/2020.08.11.245993</t>
-  </si>
-  <si>
-    <t xml:space="preserve">A SARS-CoV-2 Vaccination Strategy Focused on Population-Scale Immunity</t>
+    <t xml:space="preserve">https://doi.org/10.1101/2020.03.13.990598</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Shotgun proteomics of SARS-CoV-2 infected cells and its application to the optimisation of whole viral particle antigen production for vaccines</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://doi.org/10.1101/2020.04.17.046193</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Microscopy-based assay for semi-quantitative detection of SARS-CoV-2 specific antibodies in human sera</t>
   </si>
   <si>
     <t xml:space="preserve">2020-06-15</t>
   </si>
   <si>
-    <t xml:space="preserve">https://doi.org/10.1101/2020.03.31.018978</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SARS-CoV2 (COVID-19) Structural/Evolution Dynamicome: Insights into functional evolution and human genomics.</t>
+    <t xml:space="preserve">https://doi.org/10.1101/2020.06.15.152587</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CD8+ T cell cross-reactivity against SARS-CoV-2 conferred by other coronavirus strains and influenza virus</t>
   </si>
   <si>
     <t xml:space="preserve">2020-05-20</t>
   </si>
   <si>
-    <t xml:space="preserve">https://doi.org/10.1101/2020.05.15.098616</t>
-  </si>
-  <si>
-    <t xml:space="preserve">COVID-19 coronavirus vaccine design using reverse vaccinology and machine learning</t>
+    <t xml:space="preserve">https://doi.org/10.1101/2020.05.20.107292</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Multi-organ Proteomic Landscape of COVID-19 Autopsies</t>
   </si>
   <si>
     <t xml:space="preserve">2020-08-19</t>
   </si>
   <si>
-    <t xml:space="preserve">https://doi.org/10.1101/2020.03.20.000141</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Inhibiting coronavirus replication in cultured cells by chemical ER stress</t>
+    <t xml:space="preserve">https://doi.org/10.1101/2020.08.16.20176065</t>
+  </si>
+  <si>
+    <t xml:space="preserve">In silico Proteome analysis of Severe acute respiratory syndrome coronavirus 2 (SARS-CoV-2)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://doi.org/10.1101/2020.05.23.104919</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Multi-pronged human protein mimicry by SARS-CoV-2 reveals bifurcating potential for MHC detection and immune evasion</t>
   </si>
   <si>
     <t xml:space="preserve">2020-06-19</t>
   </si>
   <si>
-    <t xml:space="preserve">https://doi.org/10.1101/2020.08.26.266304</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Relevance of enriched expression of SARS-CoV-2 binding receptor ACE2 in gastrointestinal tissue with pathogenesis of digestive symptoms, diabetes-associated mortality, and disease recurrence in COVID-19 patients</t>
+    <t xml:space="preserve">https://doi.org/10.1101/2020.06.19.161620</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Systematic modeling of SARS-CoV-2 protein structures</t>
   </si>
   <si>
     <t xml:space="preserve">2020-07-17</t>
   </si>
   <si>
-    <t xml:space="preserve">https://doi.org/10.1101/2020.04.14.040204</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Global profiling of SARS-CoV-2 specific IgG/ IgM responses of convalescents using a proteome microarray</t>
+    <t xml:space="preserve">https://doi.org/10.1101/2020.07.16.207308</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Citizen Scientists Create an Exascale Computer to Combat COVID-19</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://doi.org/10.1101/2020.06.27.175430</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Modeling of Severe Acute Respiratory Syndrome Coronavirus 2 (SARS-CoV-2) Proteins by Machine Learning and Physics-Based Refinement</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://doi.org/10.1101/2020.03.25.008904</t>
+  </si>
+  <si>
+    <t xml:space="preserve">rSWeeP: A R/Bioconductor package deal with SWeeP sequences representation</t>
   </si>
   <si>
     <t xml:space="preserve">2020-09-10</t>
   </si>
   <si>
-    <t xml:space="preserve">https://doi.org/10.1101/2020.03.20.20039495</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Dark proteome of Newly Emerged SARS-CoV-2 in Comparison with Human and Bat Coronaviruses</t>
+    <t xml:space="preserve">https://doi.org/10.1101/2020.09.09.290247</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Human leukocyte antigen susceptibility map for SARS-CoV-2</t>
   </si>
   <si>
     <t xml:space="preserve">2020-03-26</t>
   </si>
   <si>
-    <t xml:space="preserve">https://doi.org/10.1101/2020.03.13.990598</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Shotgun proteomics of SARS-CoV-2 infected cells and its application to the optimisation of whole viral particle antigen production for vaccines</t>
+    <t xml:space="preserve">https://doi.org/10.1101/2020.03.22.20040600</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Urine Proteome of COVID-19 Patients</t>
   </si>
   <si>
     <t xml:space="preserve">2020-05-06</t>
   </si>
   <si>
-    <t xml:space="preserve">https://doi.org/10.1101/2020.04.17.046193</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Microscopy-based assay for semi-quantitative detection of SARS-CoV-2 specific antibodies in human sera</t>
+    <t xml:space="preserve">https://doi.org/10.1101/2020.05.02.20088666</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SARS-CoV-2 3CLpro Whole Human Proteome Cleavage Prediction and Enrichment/Depletion Analysis</t>
   </si>
   <si>
     <t xml:space="preserve">2020-08-25</t>
   </si>
   <si>
-    <t xml:space="preserve">https://doi.org/10.1101/2020.06.15.152587</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CD8+ T cell cross-reactivity against SARS-CoV-2 conferred by other coronavirus strains and influenza virus</t>
+    <t xml:space="preserve">https://doi.org/10.1101/2020.08.24.265645</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The aging transcriptome and cellular landscape of the human lung in relation to SARS-CoV-2</t>
   </si>
   <si>
     <t xml:space="preserve">2020-04-09</t>
   </si>
   <si>
-    <t xml:space="preserve">https://doi.org/10.1101/2020.05.20.107292</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Multi-organ Proteomic Landscape of COVID-19 Autopsies</t>
+    <t xml:space="preserve">https://doi.org/10.1101/2020.04.07.030684</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Vulnerabilities of the SARS-CoV-2 virus to proteotoxicity -- opportunity for repurposed chemotherapy of COVID-19 infection</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://doi.org/10.1101/2020.04.07.029488</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A direct RNA-protein interaction atlas of the SARS-CoV-2 RNA in infected human cells</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://doi.org/10.1101/2020.07.15.204404</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Identification of Immune complement function as a determinant of adverse SARS-CoV-2 infection outcome</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://doi.org/10.1101/2020.05.05.20092452</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Computationally validated SARS-CoV-2 CTL and HTL Multi-Patch Vaccines designed by reverse epitomics approach, shows potential to cover large ethnically distributed human population worldwide</t>
   </si>
   <si>
     <t xml:space="preserve">2020-09-06</t>
   </si>
   <si>
-    <t xml:space="preserve">https://doi.org/10.1101/2020.08.16.20176065</t>
-  </si>
-  <si>
-    <t xml:space="preserve">In silico Proteome analysis of Severe acute respiratory syndrome coronavirus 2 (SARS-CoV-2)</t>
+    <t xml:space="preserve">https://doi.org/10.1101/2020.09.06.284992</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Functional and druggability analysis of the SARS-CoV-2 proteome</t>
   </si>
   <si>
     <t xml:space="preserve">2020-08-22</t>
   </si>
   <si>
-    <t xml:space="preserve">https://doi.org/10.1101/2020.05.23.104919</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Multi-pronged human protein mimicry by SARS-CoV-2 reveals bifurcating potential for MHC detection and immune evasion</t>
+    <t xml:space="preserve">https://doi.org/10.1101/2020.08.21.261404</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Scrutinizing the SARS-CoV-2 protein information for the designing an effective vaccine encompassing both the T-cell and B-cell epitopes</t>
   </si>
   <si>
     <t xml:space="preserve">2020-04-01</t>
   </si>
   <si>
-    <t xml:space="preserve">https://doi.org/10.1101/2020.06.19.161620</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Systematic modeling of SARS-CoV-2 protein structures</t>
+    <t xml:space="preserve">https://doi.org/10.1101/2020.03.26.009209</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A SARS-CoV-2 - host proximity interactome</t>
   </si>
   <si>
     <t xml:space="preserve">2020-09-04</t>
   </si>
   <si>
-    <t xml:space="preserve">https://doi.org/10.1101/2020.07.16.207308</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Citizen Scientists Create an Exascale Computer to Combat COVID-19</t>
+    <t xml:space="preserve">https://doi.org/10.1101/2020.09.03.282103</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Compositional Variability and Mutation Spectra of Monophyletic SARS-CoV-2 Clades</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://doi.org/10.1101/2020.08.26.267781</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CETSA MS profiling for a comparative assessment of FDA approved antivirals repurposed for COVID-19 therapy identifies Trip13 as a Remdesivir off-target</t>
   </si>
   <si>
     <t xml:space="preserve">2020-07-20</t>
   </si>
   <si>
-    <t xml:space="preserve">https://doi.org/10.1101/2020.06.27.175430</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Modeling of Severe Acute Respiratory Syndrome Coronavirus 2 (SARS-CoV-2) Proteins by Machine Learning and Physics-Based Refinement</t>
+    <t xml:space="preserve">https://doi.org/10.1101/2020.07.19.210492</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SARS-CoV2 spike protein displays biologically significant similarities with paramyxovirus surface proteins; a bioinformatics study</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://doi.org/10.1101/2020.07.20.210534</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Multi-Omics integration analysis of respiratory specimen characterizes baseline molecular determinants associated with COVID-19 diagnosis.</t>
   </si>
   <si>
     <t xml:space="preserve">2020-07-07</t>
   </si>
   <si>
-    <t xml:space="preserve">https://doi.org/10.1101/2020.03.25.008904</t>
-  </si>
-  <si>
-    <t xml:space="preserve">rSWeeP: A R/Bioconductor package deal with SWeeP sequences representation</t>
+    <t xml:space="preserve">https://doi.org/10.1101/2020.07.06.20147082</t>
+  </si>
+  <si>
+    <t xml:space="preserve">In-depth blood proteome profiling analysis revealed distinct functional characteristics of plasma proteins between severe and non-severe COVID-19 patients</t>
   </si>
   <si>
     <t xml:space="preserve">2020-08-18</t>
   </si>
   <si>
-    <t xml:space="preserve">https://doi.org/10.1101/2020.09.09.290247</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Human leukocyte antigen susceptibility map for SARS-CoV-2</t>
+    <t xml:space="preserve">https://doi.org/10.1101/2020.08.18.255315</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Architecture and self-assembly of the SARS-CoV-2 nucleocapsid protein</t>
   </si>
   <si>
     <t xml:space="preserve">2020-05-17</t>
   </si>
   <si>
-    <t xml:space="preserve">https://doi.org/10.1101/2020.03.22.20040600</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Urine Proteome of COVID-19 Patients</t>
+    <t xml:space="preserve">https://doi.org/10.1101/2020.05.17.100685</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Deducing the N- and O- glycosylation profile of the spike protein of novel coronavirus SARS-CoV-2</t>
   </si>
   <si>
     <t xml:space="preserve">2020-04-03</t>
   </si>
   <si>
-    <t xml:space="preserve">https://doi.org/10.1101/2020.05.02.20088666</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SARS-CoV-2 3CLpro Whole Human Proteome Cleavage Prediction and Enrichment/Depletion Analysis</t>
+    <t xml:space="preserve">https://doi.org/10.1101/2020.04.01.020966</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SARS CoV-2 nucleocapsid protein forms condensates with viral genomic RNA</t>
   </si>
   <si>
     <t xml:space="preserve">2020-09-14</t>
   </si>
   <si>
-    <t xml:space="preserve">https://doi.org/10.1101/2020.08.24.265645</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The aging transcriptome and cellular landscape of the human lung in relation to SARS-CoV-2</t>
+    <t xml:space="preserve">https://doi.org/10.1101/2020.09.14.295824</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The Coronavirus Network Explorer: Mining a large-scale knowledge graph for effects of SARS-CoV-2 on host cell function</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://doi.org/10.1101/2020.09.14.296327</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A Combined approach of MALDI-TOF Mass Spectrometry and multivariate analysis as a potential tool for the detection of SARS-CoV-2 virus in nasopharyngeal swabs.</t>
   </si>
   <si>
     <t xml:space="preserve">2020-05-07</t>
   </si>
   <si>
-    <t xml:space="preserve">https://doi.org/10.1101/2020.04.07.030684</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Vulnerabilities of the SARS-CoV-2 virus to proteotoxicity -- opportunity for repurposed chemotherapy of COVID-19 infection</t>
+    <t xml:space="preserve">https://doi.org/10.1101/2020.05.07.082925</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cryo-EM Structures of the SARS-CoV-2 Endoribonuclease Nsp15</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://doi.org/10.1101/2020.08.11.244863</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mass Spectrometric Identification of SARS-CoV-2 Proteins from Gargle Solution Samples of COVID-19 Patients</t>
   </si>
   <si>
     <t xml:space="preserve">2020-04-19</t>
   </si>
   <si>
-    <t xml:space="preserve">https://doi.org/10.1101/2020.04.07.029488</t>
-  </si>
-  <si>
-    <t xml:space="preserve">A direct RNA-protein interaction atlas of the SARS-CoV-2 RNA in infected human cells</t>
+    <t xml:space="preserve">https://doi.org/10.1101/2020.04.18.047878</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Crystallographic and electrophilic fragment screening of the SARS-CoV-2 main protease</t>
   </si>
   <si>
     <t xml:space="preserve">2020-05-27</t>
   </si>
   <si>
-    <t xml:space="preserve">https://doi.org/10.1101/2020.07.15.204404</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Identification of Immune complement function as a determinant of adverse SARS-CoV-2 infection outcome</t>
+    <t xml:space="preserve">https://doi.org/10.1101/2020.05.27.118117</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Characterisation of the transcriptome and proteome of SARS-CoV-2 using direct RNA sequencing and tandem mass spectrometry reveals evidence for a cell passage induced in-frame deletion in the spike glycoprotein that removes the furin-like cleavage site.</t>
   </si>
   <si>
     <t xml:space="preserve">2020-03-24</t>
   </si>
   <si>
-    <t xml:space="preserve">https://doi.org/10.1101/2020.05.05.20092452</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Computationally validated SARS-CoV-2 CTL and HTL Multi-Patch Vaccines designed by reverse epitomics approach, shows potential to cover large ethnically distributed human population worldwide</t>
+    <t xml:space="preserve">https://doi.org/10.1101/2020.03.22.002204</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Boceprevir, GC-376, and calpain inhibitors II, XII inhibit SARS-CoV-2 viral replication by targeting the viral main protease</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://doi.org/10.1101/2020.04.20.051581</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A SARS-CoV-2-Human Protein-Protein Interaction Map Reveals Drug Targets and Potential Drug-Repurposing</t>
   </si>
   <si>
     <t xml:space="preserve">2020-03-22</t>
   </si>
   <si>
-    <t xml:space="preserve">https://doi.org/10.1101/2020.09.06.284992</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Functional and druggability analysis of the SARS-CoV-2 proteome</t>
+    <t xml:space="preserve">https://doi.org/10.1101/2020.03.22.002386</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The utility of native MS for understanding the mechanism of action of repurposed therapeutics in COVID-19: heparin as a disruptor of the SARS-CoV-2 interaction with its host cell receptor.</t>
   </si>
   <si>
     <t xml:space="preserve">2020-06-10</t>
   </si>
   <si>
-    <t xml:space="preserve">https://doi.org/10.1101/2020.08.21.261404</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Scrutinizing the SARS-CoV-2 protein information for the designing an effective vaccine encompassing both the T-cell and B-cell epitopes</t>
+    <t xml:space="preserve">https://doi.org/10.1101/2020.06.09.142794</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Celebrex adjuvant therapy on COVID-19: An experimental study</t>
   </si>
   <si>
     <t xml:space="preserve">2020-05-11</t>
   </si>
   <si>
-    <t xml:space="preserve">https://doi.org/10.1101/2020.03.26.009209</t>
-  </si>
-  <si>
-    <t xml:space="preserve">A SARS-CoV-2 - host proximity interactome</t>
+    <t xml:space="preserve">https://doi.org/10.1101/2020.05.05.20077610</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Allosteric inhibition of the SARS-CoV-2 main protease - insights from mass spectrometry-based assays</t>
   </si>
   <si>
     <t xml:space="preserve">2020-07-29</t>
   </si>
   <si>
-    <t xml:space="preserve">https://doi.org/10.1101/2020.09.03.282103</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Compositional Variability and Mutation Spectra of Monophyletic SARS-CoV-2 Clades</t>
+    <t xml:space="preserve">https://doi.org/10.1101/2020.07.29.226761</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Production of Trimeric SARS-CoV-2 Spike Protein by CHO Cells for Serological COVID-19 Testing</t>
   </si>
   <si>
     <t xml:space="preserve">2020-08-13</t>
   </si>
   <si>
-    <t xml:space="preserve">https://doi.org/10.1101/2020.08.26.267781</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CETSA MS profiling for a comparative assessment of FDA approved antivirals repurposed for COVID-19 therapy identifies Trip13 as a Remdesivir off-target</t>
+    <t xml:space="preserve">https://doi.org/10.1101/2020.08.07.20169441</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Site-specific N-glycosylation Characterization of Recombinant SARS-CoV-2 Spike Proteins using High-Resolution Mass Spectrometry</t>
   </si>
   <si>
     <t xml:space="preserve">2020-03-29</t>
   </si>
   <si>
-    <t xml:space="preserve">https://doi.org/10.1101/2020.07.19.210492</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SARS-CoV2 spike protein displays biologically significant similarities with paramyxovirus surface proteins; a bioinformatics study</t>
+    <t xml:space="preserve">https://doi.org/10.1101/2020.03.28.013276</t>
+  </si>
+  <si>
+    <t xml:space="preserve">N-glycosylation network construction and analysis to modify glycans on the spike S glycoprotein of SARS-CoV-2.</t>
   </si>
   <si>
     <t xml:space="preserve">2020-06-24</t>
   </si>
   <si>
-    <t xml:space="preserve">https://doi.org/10.1101/2020.07.20.210534</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Multi-Omics integration analysis of respiratory specimen characterizes baseline molecular determinants associated with COVID-19 diagnosis.</t>
+    <t xml:space="preserve">https://doi.org/10.1101/2020.06.23.167791</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mucin-type O-glycosylation Landscapes of SARS-CoV-2 Spike Proteins</t>
   </si>
   <si>
     <t xml:space="preserve">2020-07-30</t>
   </si>
   <si>
-    <t xml:space="preserve">https://doi.org/10.1101/2020.07.06.20147082</t>
-  </si>
-  <si>
-    <t xml:space="preserve">In-depth blood proteome profiling analysis revealed distinct functional characteristics of plasma proteins between severe and non-severe COVID-19 patients</t>
+    <t xml:space="preserve">https://doi.org/10.1101/2020.07.29.227785</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Proteotyping SARS-CoV-2 virus from nasopharyngeal swabs: a proof-of-concept focused on a 3 min mass spectrometry window</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://doi.org/10.1101/2020.06.19.161000</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Covid-19 automated diagnosis and risk assessment through Metabolomics and Machine-Learning</t>
   </si>
   <si>
     <t xml:space="preserve">2020-07-27</t>
   </si>
   <si>
-    <t xml:space="preserve">https://doi.org/10.1101/2020.08.18.255315</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Architecture and self-assembly of the SARS-CoV-2 nucleocapsid protein</t>
+    <t xml:space="preserve">https://doi.org/10.1101/2020.07.24.20161828</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A clinical MALDI-ToF Mass spectrometry assay for SARS-CoV-2: Rational design and multi-disciplinary team work.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://doi.org/10.1101/2020.08.22.20176669</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Development of mass spectrometry-based targeted assay for direct detection of novel SARS-CoV-2 coronavirus from clinical specimens</t>
   </si>
   <si>
     <t xml:space="preserve">2020-08-06</t>
   </si>
   <si>
-    <t xml:space="preserve">https://doi.org/10.1101/2020.05.17.100685</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Deducing the N- and O- glycosylation profile of the spike protein of novel coronavirus SARS-CoV-2</t>
+    <t xml:space="preserve">https://doi.org/10.1101/2020.08.05.20168948</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TARGETED PROTEOMICS FOR THE DETECTION OF SARS-COV-2 PROTEINS.</t>
   </si>
   <si>
     <t xml:space="preserve">2020-04-23</t>
   </si>
   <si>
-    <t xml:space="preserve">https://doi.org/10.1101/2020.04.01.020966</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SARS CoV-2 nucleocapsid protein forms condensates with viral genomic RNA</t>
+    <t xml:space="preserve">https://doi.org/10.1101/2020.04.23.057810</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Large-scale Multi-omic Analysis of COVID-19 Severity</t>
   </si>
   <si>
     <t xml:space="preserve">2020-07-19</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://doi.org/10.1101/2020.09.14.295824</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The Coronavirus Network Explorer: Mining a large-scale knowledge graph for effects of SARS-CoV-2 on host cell function</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://doi.org/10.1101/2020.09.14.296327</t>
-  </si>
-  <si>
-    <t xml:space="preserve">A Combined approach of MALDI-TOF Mass Spectrometry and multivariate analysis as a potential tool for the detection of SARS-CoV-2 virus in nasopharyngeal swabs.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://doi.org/10.1101/2020.05.07.082925</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Cryo-EM Structures of the SARS-CoV-2 Endoribonuclease Nsp15</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://doi.org/10.1101/2020.08.11.244863</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mass Spectrometric Identification of SARS-CoV-2 Proteins from Gargle Solution Samples of COVID-19 Patients</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://doi.org/10.1101/2020.04.18.047878</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Crystallographic and electrophilic fragment screening of the SARS-CoV-2 main protease</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://doi.org/10.1101/2020.05.27.118117</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Characterisation of the transcriptome and proteome of SARS-CoV-2 using direct RNA sequencing and tandem mass spectrometry reveals evidence for a cell passage induced in-frame deletion in the spike glycoprotein that removes the furin-like cleavage site.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://doi.org/10.1101/2020.03.22.002204</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Boceprevir, GC-376, and calpain inhibitors II, XII inhibit SARS-CoV-2 viral replication by targeting the viral main protease</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://doi.org/10.1101/2020.04.20.051581</t>
-  </si>
-  <si>
-    <t xml:space="preserve">A SARS-CoV-2-Human Protein-Protein Interaction Map Reveals Drug Targets and Potential Drug-Repurposing</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://doi.org/10.1101/2020.03.22.002386</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The utility of native MS for understanding the mechanism of action of repurposed therapeutics in COVID-19: heparin as a disruptor of the SARS-CoV-2 interaction with its host cell receptor.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://doi.org/10.1101/2020.06.09.142794</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Celebrex adjuvant therapy on COVID-19: An experimental study</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://doi.org/10.1101/2020.05.05.20077610</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Allosteric inhibition of the SARS-CoV-2 main protease - insights from mass spectrometry-based assays</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://doi.org/10.1101/2020.07.29.226761</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Production of Trimeric SARS-CoV-2 Spike Protein by CHO Cells for Serological COVID-19 Testing</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://doi.org/10.1101/2020.08.07.20169441</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Site-specific N-glycosylation Characterization of Recombinant SARS-CoV-2 Spike Proteins using High-Resolution Mass Spectrometry</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://doi.org/10.1101/2020.03.28.013276</t>
-  </si>
-  <si>
-    <t xml:space="preserve">N-glycosylation network construction and analysis to modify glycans on the spike S glycoprotein of SARS-CoV-2.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://doi.org/10.1101/2020.06.23.167791</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mucin-type O-glycosylation Landscapes of SARS-CoV-2 Spike Proteins</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://doi.org/10.1101/2020.07.29.227785</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Proteotyping SARS-CoV-2 virus from nasopharyngeal swabs: a proof-of-concept focused on a 3 min mass spectrometry window</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://doi.org/10.1101/2020.06.19.161000</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Covid-19 automated diagnosis and risk assessment through Metabolomics and Machine-Learning</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://doi.org/10.1101/2020.07.24.20161828</t>
-  </si>
-  <si>
-    <t xml:space="preserve">A clinical MALDI-ToF Mass spectrometry assay for SARS-CoV-2: Rational design and multi-disciplinary team work.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://doi.org/10.1101/2020.08.22.20176669</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Development of mass spectrometry-based targeted assay for direct detection of novel SARS-CoV-2 coronavirus from clinical specimens</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://doi.org/10.1101/2020.08.05.20168948</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TARGETED PROTEOMICS FOR THE DETECTION OF SARS-COV-2 PROTEINS.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://doi.org/10.1101/2020.04.23.057810</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Large-scale Multi-omic Analysis of COVID-19 Severity</t>
   </si>
   <si>
     <t xml:space="preserve">https://doi.org/10.1101/2020.07.17.20156513</t>
@@ -896,7 +896,7 @@
   </sheetPr>
   <dimension ref="A1:C93"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A46" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
@@ -989,878 +989,941 @@
         <v>21</v>
       </c>
       <c r="B8" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C8" s="0" t="s">
         <v>22</v>
-      </c>
-      <c r="C8" s="0" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="B9" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B9" s="1" t="s">
+      <c r="C9" s="0" t="s">
         <v>25</v>
-      </c>
-      <c r="C9" s="0" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="B10" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="B10" s="1" t="s">
+      <c r="C10" s="0" t="s">
         <v>28</v>
-      </c>
-      <c r="C10" s="0" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="B11" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="B11" s="1" t="s">
+      <c r="C11" s="0" t="s">
         <v>31</v>
-      </c>
-      <c r="C11" s="0" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="B12" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="B12" s="1" t="s">
+      <c r="C12" s="0" t="s">
         <v>34</v>
-      </c>
-      <c r="C12" s="0" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C13" s="0" t="s">
         <v>36</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="C13" s="0" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C14" s="0" t="s">
         <v>39</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="C14" s="0" t="s">
-        <v>41</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
+        <v>40</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="C15" s="0" t="s">
         <v>42</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="C15" s="0" t="s">
-        <v>44</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="C16" s="0" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="C17" s="0" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="C18" s="0" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="C19" s="0" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="C20" s="0" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="C21" s="0" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="C22" s="0" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="C23" s="0" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="C24" s="0" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="C25" s="0" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="C26" s="0" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="C27" s="0" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="C28" s="0" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>85</v>
+        <v>16</v>
       </c>
       <c r="C29" s="0" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="C30" s="0" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>91</v>
+        <v>7</v>
       </c>
       <c r="C31" s="0" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>94</v>
+        <v>61</v>
       </c>
       <c r="C32" s="0" t="s">
-        <v>95</v>
+        <v>89</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="C33" s="0" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
       <c r="C34" s="0" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="s">
-        <v>102</v>
+        <v>96</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="C35" s="0" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="0" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
       <c r="C36" s="0" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="0" t="s">
-        <v>108</v>
+        <v>102</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>109</v>
+        <v>13</v>
       </c>
       <c r="C37" s="0" t="s">
-        <v>110</v>
+        <v>103</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="0" t="s">
-        <v>111</v>
+        <v>104</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>112</v>
+        <v>105</v>
       </c>
       <c r="C38" s="0" t="s">
-        <v>113</v>
+        <v>106</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="0" t="s">
-        <v>114</v>
+        <v>107</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>115</v>
+        <v>108</v>
       </c>
       <c r="C39" s="0" t="s">
-        <v>116</v>
+        <v>109</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="0" t="s">
-        <v>117</v>
+        <v>110</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>118</v>
+        <v>111</v>
       </c>
       <c r="C40" s="0" t="s">
-        <v>119</v>
+        <v>112</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="0" t="s">
-        <v>120</v>
+        <v>113</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>121</v>
+        <v>114</v>
       </c>
       <c r="C41" s="0" t="s">
-        <v>122</v>
+        <v>115</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="0" t="s">
-        <v>123</v>
+        <v>116</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>124</v>
+        <v>117</v>
       </c>
       <c r="C42" s="0" t="s">
-        <v>125</v>
+        <v>118</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="0" t="s">
-        <v>126</v>
+        <v>119</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>127</v>
+        <v>120</v>
       </c>
       <c r="C43" s="0" t="s">
-        <v>128</v>
+        <v>121</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="0" t="s">
-        <v>129</v>
+        <v>122</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>130</v>
+        <v>70</v>
       </c>
       <c r="C44" s="0" t="s">
-        <v>131</v>
+        <v>123</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="0" t="s">
-        <v>132</v>
+        <v>124</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>133</v>
+        <v>125</v>
       </c>
       <c r="C45" s="0" t="s">
-        <v>134</v>
+        <v>126</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="0" t="s">
-        <v>135</v>
+        <v>127</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>136</v>
+        <v>128</v>
       </c>
       <c r="C46" s="0" t="s">
-        <v>137</v>
+        <v>129</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="0" t="s">
-        <v>138</v>
+        <v>130</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>139</v>
+        <v>131</v>
       </c>
       <c r="C47" s="0" t="s">
-        <v>140</v>
+        <v>132</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="0" t="s">
-        <v>141</v>
+        <v>133</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>142</v>
+        <v>24</v>
       </c>
       <c r="C48" s="0" t="s">
-        <v>143</v>
+        <v>134</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="0" t="s">
-        <v>144</v>
+        <v>135</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>145</v>
+        <v>136</v>
       </c>
       <c r="C49" s="0" t="s">
-        <v>146</v>
+        <v>137</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="0" t="s">
-        <v>147</v>
+        <v>138</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>148</v>
+        <v>139</v>
       </c>
       <c r="C50" s="0" t="s">
-        <v>149</v>
+        <v>140</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="0" t="s">
-        <v>150</v>
+        <v>141</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>151</v>
+        <v>38</v>
       </c>
       <c r="C51" s="0" t="s">
-        <v>152</v>
+        <v>142</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="0" t="s">
-        <v>153</v>
+        <v>143</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>154</v>
+        <v>41</v>
       </c>
       <c r="C52" s="0" t="s">
-        <v>155</v>
+        <v>144</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="0" t="s">
-        <v>156</v>
+        <v>145</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>157</v>
+        <v>146</v>
       </c>
       <c r="C53" s="0" t="s">
-        <v>158</v>
+        <v>147</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="0" t="s">
-        <v>159</v>
+        <v>148</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>160</v>
+        <v>149</v>
       </c>
       <c r="C54" s="0" t="s">
-        <v>161</v>
+        <v>150</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="0" t="s">
-        <v>162</v>
+        <v>151</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>163</v>
+        <v>152</v>
       </c>
       <c r="C55" s="0" t="s">
-        <v>164</v>
+        <v>153</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="0" t="s">
-        <v>165</v>
+        <v>154</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>166</v>
+        <v>155</v>
       </c>
       <c r="C56" s="0" t="s">
-        <v>167</v>
+        <v>156</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="0" t="s">
-        <v>168</v>
+        <v>157</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>169</v>
+        <v>158</v>
       </c>
       <c r="C57" s="0" t="s">
-        <v>170</v>
+        <v>159</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="0" t="s">
-        <v>171</v>
+        <v>160</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>172</v>
+        <v>158</v>
       </c>
       <c r="C58" s="0" t="s">
-        <v>173</v>
+        <v>161</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="0" t="s">
-        <v>174</v>
+        <v>162</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>175</v>
+        <v>27</v>
       </c>
       <c r="C59" s="0" t="s">
-        <v>176</v>
+        <v>163</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="0" t="s">
-        <v>177</v>
+        <v>164</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>178</v>
+        <v>61</v>
       </c>
       <c r="C60" s="0" t="s">
-        <v>179</v>
+        <v>165</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="0" t="s">
-        <v>180</v>
+        <v>166</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>181</v>
+        <v>167</v>
       </c>
       <c r="C61" s="0" t="s">
-        <v>182</v>
+        <v>168</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="0" t="s">
-        <v>183</v>
+        <v>169</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>184</v>
+        <v>170</v>
       </c>
       <c r="C62" s="0" t="s">
-        <v>185</v>
+        <v>171</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="0" t="s">
-        <v>186</v>
+        <v>172</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>187</v>
+        <v>173</v>
       </c>
       <c r="C63" s="0" t="s">
-        <v>188</v>
+        <v>174</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="0" t="s">
-        <v>189</v>
+        <v>175</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>190</v>
+        <v>176</v>
       </c>
       <c r="C64" s="0" t="s">
-        <v>191</v>
+        <v>177</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="0" t="s">
-        <v>192</v>
+        <v>178</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>193</v>
+        <v>64</v>
       </c>
       <c r="C65" s="0" t="s">
-        <v>194</v>
+        <v>179</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="0" t="s">
-        <v>195</v>
+        <v>180</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>196</v>
+        <v>181</v>
       </c>
       <c r="C66" s="0" t="s">
-        <v>197</v>
+        <v>182</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="0" t="s">
-        <v>198</v>
+        <v>183</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>199</v>
+        <v>181</v>
       </c>
       <c r="C67" s="0" t="s">
-        <v>200</v>
+        <v>184</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="0" t="s">
-        <v>201</v>
+        <v>185</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>202</v>
+        <v>186</v>
       </c>
       <c r="C68" s="0" t="s">
-        <v>203</v>
+        <v>187</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="0" t="s">
-        <v>204</v>
+        <v>188</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>205</v>
+        <v>189</v>
       </c>
       <c r="C69" s="0" t="s">
-        <v>206</v>
+        <v>190</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="0" t="s">
-        <v>207</v>
+        <v>191</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>208</v>
+        <v>192</v>
       </c>
       <c r="C70" s="0" t="s">
-        <v>209</v>
+        <v>193</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="0" t="s">
-        <v>210</v>
+        <v>194</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>211</v>
+        <v>195</v>
       </c>
       <c r="C71" s="0" t="s">
-        <v>212</v>
+        <v>196</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="0" t="s">
-        <v>213</v>
+        <v>197</v>
       </c>
       <c r="B72" s="1" t="s">
-        <v>214</v>
+        <v>198</v>
       </c>
       <c r="C72" s="0" t="s">
-        <v>215</v>
+        <v>199</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="0" t="s">
-        <v>216</v>
+        <v>200</v>
+      </c>
+      <c r="B73" s="1" t="s">
+        <v>198</v>
       </c>
       <c r="C73" s="0" t="s">
-        <v>217</v>
+        <v>201</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="0" t="s">
-        <v>218</v>
+        <v>202</v>
+      </c>
+      <c r="B74" s="1" t="s">
+        <v>203</v>
       </c>
       <c r="C74" s="0" t="s">
-        <v>219</v>
+        <v>204</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="0" t="s">
-        <v>220</v>
+        <v>205</v>
+      </c>
+      <c r="B75" s="1" t="s">
+        <v>100</v>
       </c>
       <c r="C75" s="0" t="s">
-        <v>221</v>
+        <v>206</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="0" t="s">
-        <v>222</v>
+        <v>207</v>
+      </c>
+      <c r="B76" s="1" t="s">
+        <v>208</v>
       </c>
       <c r="C76" s="0" t="s">
-        <v>223</v>
+        <v>209</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="0" t="s">
-        <v>224</v>
+        <v>210</v>
+      </c>
+      <c r="B77" s="1" t="s">
+        <v>211</v>
       </c>
       <c r="C77" s="0" t="s">
-        <v>225</v>
+        <v>212</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="0" t="s">
-        <v>226</v>
+        <v>213</v>
+      </c>
+      <c r="B78" s="1" t="s">
+        <v>214</v>
       </c>
       <c r="C78" s="0" t="s">
-        <v>227</v>
+        <v>215</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A79" s="0" t="s">
-        <v>228</v>
+        <v>216</v>
+      </c>
+      <c r="B79" s="1" t="s">
+        <v>97</v>
       </c>
       <c r="C79" s="0" t="s">
-        <v>229</v>
+        <v>217</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A80" s="0" t="s">
-        <v>230</v>
+        <v>218</v>
+      </c>
+      <c r="B80" s="1" t="s">
+        <v>219</v>
       </c>
       <c r="C80" s="0" t="s">
-        <v>231</v>
+        <v>220</v>
       </c>
     </row>
     <row r="81" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A81" s="0" t="s">
-        <v>232</v>
+        <v>221</v>
+      </c>
+      <c r="B81" s="1" t="s">
+        <v>222</v>
       </c>
       <c r="C81" s="0" t="s">
-        <v>233</v>
+        <v>223</v>
       </c>
     </row>
     <row r="82" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A82" s="0" t="s">
-        <v>234</v>
+        <v>224</v>
+      </c>
+      <c r="B82" s="1" t="s">
+        <v>225</v>
       </c>
       <c r="C82" s="0" t="s">
-        <v>235</v>
+        <v>226</v>
       </c>
     </row>
     <row r="83" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A83" s="0" t="s">
-        <v>236</v>
+        <v>227</v>
+      </c>
+      <c r="B83" s="1" t="s">
+        <v>228</v>
       </c>
       <c r="C83" s="0" t="s">
-        <v>237</v>
+        <v>229</v>
       </c>
     </row>
     <row r="84" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A84" s="0" t="s">
-        <v>238</v>
+        <v>230</v>
+      </c>
+      <c r="B84" s="1" t="s">
+        <v>231</v>
       </c>
       <c r="C84" s="0" t="s">
-        <v>239</v>
+        <v>232</v>
       </c>
     </row>
     <row r="85" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A85" s="0" t="s">
-        <v>240</v>
+        <v>233</v>
+      </c>
+      <c r="B85" s="1" t="s">
+        <v>234</v>
       </c>
       <c r="C85" s="0" t="s">
-        <v>241</v>
+        <v>235</v>
       </c>
     </row>
     <row r="86" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A86" s="0" t="s">
-        <v>242</v>
+        <v>236</v>
+      </c>
+      <c r="B86" s="1" t="s">
+        <v>237</v>
       </c>
       <c r="C86" s="0" t="s">
-        <v>243</v>
+        <v>238</v>
       </c>
     </row>
     <row r="87" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A87" s="0" t="s">
-        <v>244</v>
+        <v>239</v>
+      </c>
+      <c r="B87" s="1" t="s">
+        <v>240</v>
       </c>
       <c r="C87" s="0" t="s">
-        <v>245</v>
+        <v>241</v>
       </c>
     </row>
     <row r="88" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A88" s="0" t="s">
-        <v>246</v>
+        <v>242</v>
+      </c>
+      <c r="B88" s="1" t="s">
+        <v>136</v>
       </c>
       <c r="C88" s="0" t="s">
-        <v>247</v>
+        <v>243</v>
       </c>
     </row>
     <row r="89" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A89" s="0" t="s">
-        <v>248</v>
+        <v>244</v>
+      </c>
+      <c r="B89" s="1" t="s">
+        <v>245</v>
       </c>
       <c r="C89" s="0" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
     </row>
     <row r="90" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A90" s="0" t="s">
-        <v>250</v>
+        <v>247</v>
+      </c>
+      <c r="B90" s="1" t="s">
+        <v>170</v>
       </c>
       <c r="C90" s="0" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
     </row>
     <row r="91" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A91" s="0" t="s">
-        <v>252</v>
+        <v>249</v>
+      </c>
+      <c r="B91" s="1" t="s">
+        <v>250</v>
       </c>
       <c r="C91" s="0" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
     </row>
     <row r="92" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A92" s="0" t="s">
+        <v>252</v>
+      </c>
+      <c r="B92" s="1" t="s">
+        <v>253</v>
+      </c>
+      <c r="C92" s="0" t="s">
         <v>254</v>
-      </c>
-      <c r="C92" s="0" t="s">
-        <v>255</v>
       </c>
     </row>
     <row r="93" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A93" s="0" t="s">
+        <v>255</v>
+      </c>
+      <c r="B93" s="1" t="s">
         <v>256</v>
       </c>
       <c r="C93" s="0" t="s">

</xml_diff>